<commit_message>
Fix for issue #11317
This includes updates to 3 Excel files, plus a test in test_excel.py,
plus the fix in parsers.py
</commit_message>
<xml_diff>
--- a/pandas/io/tests/data/testmultiindex.xlsx
+++ b/pandas/io/tests/data/testmultiindex.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris\Documents\python-dev\pandas\pandas\io\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anaconda3\Lib\site-packages\pandas\io\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="single_column_name" sheetId="9" r:id="rId1"/>
@@ -17,16 +17,20 @@
     <sheet name="mi_index" sheetId="5" r:id="rId3"/>
     <sheet name="both" sheetId="6" r:id="rId4"/>
     <sheet name="mi_column_name" sheetId="4" r:id="rId5"/>
-    <sheet name="mi_index_name" sheetId="7" r:id="rId6"/>
-    <sheet name="both_name" sheetId="8" r:id="rId7"/>
-    <sheet name="both_name_skiprows" sheetId="10" r:id="rId8"/>
+    <sheet name="name_with_int" sheetId="12" r:id="rId6"/>
+    <sheet name="mi_index_name" sheetId="7" r:id="rId7"/>
+    <sheet name="both_name" sheetId="8" r:id="rId8"/>
+    <sheet name="both_name_skiprows" sheetId="10" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="124519" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="10">
   <si>
     <t>a</t>
   </si>
@@ -117,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -150,12 +154,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -457,7 +492,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,14 +599,14 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="11"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -782,14 +817,14 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="5"/>
-      <c r="C1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="11"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>
@@ -807,7 +842,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -827,7 +862,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -845,7 +880,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -865,7 +900,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="5" t="s">
         <v>1</v>
       </c>
@@ -907,14 +942,14 @@
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="11"/>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1012,9 +1047,126 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11">
+        <v>2</v>
+      </c>
+      <c r="D2" s="11">
+        <v>1</v>
+      </c>
+      <c r="E2" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="11">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2.5</v>
+      </c>
+      <c r="D3" s="2">
+        <v>42005</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3.5</v>
+      </c>
+      <c r="D4" s="2">
+        <v>42006</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>4.5</v>
+      </c>
+      <c r="D5" s="2">
+        <v>42007</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>5.5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>42008</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:F5"/>
     </sheetView>
   </sheetViews>
@@ -1041,7 +1193,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1061,7 +1213,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1079,7 +1231,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1099,7 +1251,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1125,7 +1277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -1139,14 +1291,14 @@
       <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="11"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -1178,7 +1330,7 @@
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1198,7 +1350,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
@@ -1216,7 +1368,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -1236,7 +1388,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
@@ -1264,7 +1416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F9"/>
   <sheetViews>
@@ -1278,14 +1430,14 @@
       <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11" t="s">
+      <c r="C3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
@@ -1317,7 +1469,7 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="9" t="s">
@@ -1337,7 +1489,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="9" t="s">
         <v>1</v>
       </c>
@@ -1355,7 +1507,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -1375,7 +1527,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="9" t="s">
         <v>1</v>
       </c>

</xml_diff>